<commit_message>
sixth update: complete 20 regions of Kalimantan (not yet run)
</commit_message>
<xml_diff>
--- a/database/calliope_generators_kalimantan.xlsx
+++ b/database/calliope_generators_kalimantan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_power_system\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0C1770-5C90-48B3-99C8-8A2C674D251A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24CA026-7046-4A0A-944B-9705F0B180A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="11748" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2214,8 +2214,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7007,19 +7008,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P464"/>
+  <dimension ref="A1:N468"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="56" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.77734375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -13767,6 +13772,9 @@
       <c r="H158" t="s">
         <v>555</v>
       </c>
+      <c r="M158">
+        <v>35</v>
+      </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
@@ -14213,6 +14221,9 @@
       <c r="H168" t="s">
         <v>555</v>
       </c>
+      <c r="M168">
+        <v>35</v>
+      </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
@@ -15342,7 +15353,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>538</v>
       </c>
@@ -15368,7 +15379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>11</v>
       </c>
@@ -15415,7 +15426,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>11</v>
       </c>
@@ -15461,7 +15472,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>11</v>
       </c>
@@ -15508,7 +15519,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -15555,7 +15566,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -15602,7 +15613,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>11</v>
       </c>
@@ -15649,7 +15660,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>11</v>
       </c>
@@ -15696,7 +15707,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>11</v>
       </c>
@@ -15713,9 +15724,6 @@
         <f>_xlfn.XLOOKUP(B201,[1]plotting_generators_substation!$L$2:$L$464,[1]plotting_generators_substation!$C$2:$C$464)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="F201">
-        <v>14</v>
-      </c>
       <c r="G201" t="s">
         <v>17</v>
       </c>
@@ -15742,11 +15750,8 @@
         <f>_xlfn.XLOOKUP(J201,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="P201">
-        <v>7.12</v>
-      </c>
-    </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -15792,7 +15797,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -15839,7 +15844,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -15886,7 +15891,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>11</v>
       </c>
@@ -15933,7 +15938,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -15980,7 +15985,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>11</v>
       </c>
@@ -16027,7 +16032,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -16073,11 +16078,8 @@
         <f>_xlfn.XLOOKUP(J208,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="P208">
-        <v>1.5840000000000001</v>
-      </c>
-    </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>11</v>
       </c>
@@ -16124,7 +16126,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>11</v>
       </c>
@@ -16171,7 +16173,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -16217,11 +16219,8 @@
         <f>_xlfn.XLOOKUP(J211,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="P211">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>11</v>
       </c>
@@ -16268,7 +16267,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>11</v>
       </c>
@@ -16315,7 +16314,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>11</v>
       </c>
@@ -16362,7 +16361,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>11</v>
       </c>
@@ -16409,7 +16408,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>11</v>
       </c>
@@ -16456,7 +16455,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>11</v>
       </c>
@@ -16502,11 +16501,8 @@
         <f>_xlfn.XLOOKUP(J217,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="P217">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -16552,11 +16548,8 @@
         <f>_xlfn.XLOOKUP(J218,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Tengah</v>
       </c>
-      <c r="P218">
-        <v>0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>11</v>
       </c>
@@ -16603,7 +16596,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -16650,7 +16643,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>11</v>
       </c>
@@ -16697,7 +16690,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>11</v>
       </c>
@@ -16744,7 +16737,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>11</v>
       </c>
@@ -16791,7 +16784,7 @@
         <v>Kalimantan Tengah</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>11</v>
       </c>
@@ -26683,6 +26676,9 @@
       <c r="H439" t="s">
         <v>549</v>
       </c>
+      <c r="M439">
+        <v>63</v>
+      </c>
     </row>
     <row r="440" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
@@ -27129,6 +27125,9 @@
       <c r="H449" t="s">
         <v>555</v>
       </c>
+      <c r="M449">
+        <v>63</v>
+      </c>
     </row>
     <row r="450" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B450" t="s">
@@ -27152,6 +27151,9 @@
       <c r="H450" t="s">
         <v>555</v>
       </c>
+      <c r="M450">
+        <v>63</v>
+      </c>
     </row>
     <row r="451" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
@@ -27316,6 +27318,9 @@
       <c r="H454" t="s">
         <v>549</v>
       </c>
+      <c r="M454">
+        <v>63</v>
+      </c>
     </row>
     <row r="455" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B455" t="s">
@@ -27339,6 +27344,9 @@
       <c r="H455" t="s">
         <v>549</v>
       </c>
+      <c r="M455">
+        <v>63</v>
+      </c>
     </row>
     <row r="456" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B456" t="s">
@@ -27362,6 +27370,9 @@
       <c r="H456" t="s">
         <v>549</v>
       </c>
+      <c r="M456">
+        <v>63</v>
+      </c>
     </row>
     <row r="457" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B457" t="s">
@@ -27385,6 +27396,9 @@
       <c r="H457" t="s">
         <v>549</v>
       </c>
+      <c r="M457">
+        <v>63</v>
+      </c>
     </row>
     <row r="458" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B458" t="s">
@@ -27408,6 +27422,9 @@
       <c r="H458" t="s">
         <v>549</v>
       </c>
+      <c r="M458">
+        <v>63</v>
+      </c>
     </row>
     <row r="459" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B459" t="s">
@@ -27431,6 +27448,9 @@
       <c r="H459" t="s">
         <v>549</v>
       </c>
+      <c r="M459">
+        <v>63</v>
+      </c>
     </row>
     <row r="460" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
@@ -27548,6 +27568,9 @@
       <c r="H462" t="s">
         <v>549</v>
       </c>
+      <c r="M462">
+        <v>63</v>
+      </c>
     </row>
     <row r="463" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
@@ -27642,6 +27665,12 @@
         <f>_xlfn.XLOOKUP(J464,[2]base_substations_kalimantan!$A$2:$A$65,[2]base_substations_kalimantan!$H$2:$H$65)</f>
         <v>Kalimantan Utara</v>
       </c>
+    </row>
+    <row r="467" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H467" s="1"/>
+    </row>
+    <row r="468" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H468" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M464" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
fourteen update: midterm fix
</commit_message>
<xml_diff>
--- a/database/calliope_generators_kalimantan.xlsx
+++ b/database/calliope_generators_kalimantan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilma\Documents\Calliope\kalimantan_energy_transition\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E105362D-569A-49EB-9488-EA9884CEDA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E39A8-C848-4F21-A0F7-0BC6C0DE251B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11724" windowHeight="12636" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -7021,11 +7021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R468"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7145,7 +7144,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -7199,7 +7198,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -7307,7 +7306,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -7361,7 +7360,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7556,7 +7555,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7664,7 +7663,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>503</v>
       </c>
@@ -7697,7 +7696,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7751,7 +7750,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -7805,7 +7804,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -7967,7 +7966,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -8021,7 +8020,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>500</v>
       </c>
@@ -8054,7 +8053,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -8174,7 +8173,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>502</v>
       </c>
@@ -8207,7 +8206,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -8423,7 +8422,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -8477,7 +8476,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -8531,7 +8530,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -8585,7 +8584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -8693,7 +8692,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -8801,7 +8800,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -8909,7 +8908,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>512</v>
       </c>
@@ -8942,7 +8941,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -8996,7 +8995,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -9050,7 +9049,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -9104,7 +9103,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -9158,7 +9157,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -9212,7 +9211,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -9320,7 +9319,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>506</v>
       </c>
@@ -9353,7 +9352,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>507</v>
       </c>
@@ -9386,7 +9385,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>508</v>
       </c>
@@ -9473,7 +9472,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -9689,7 +9688,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -9742,7 +9741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -10066,7 +10065,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -10120,7 +10119,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -10174,7 +10173,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -10261,7 +10260,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>515</v>
       </c>
@@ -10294,7 +10293,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>514</v>
       </c>
@@ -10327,7 +10326,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>516</v>
       </c>
@@ -10360,7 +10359,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -10414,7 +10413,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>509</v>
       </c>
@@ -10447,7 +10446,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>511</v>
       </c>
@@ -10696,7 +10695,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>510</v>
       </c>
@@ -10783,7 +10782,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -10870,7 +10869,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -10957,7 +10956,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -11011,7 +11010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -11260,7 +11259,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -11368,7 +11367,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -11422,7 +11421,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -11476,7 +11475,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -11530,7 +11529,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -11584,7 +11583,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>518</v>
       </c>
@@ -11617,7 +11616,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>519</v>
       </c>
@@ -11650,7 +11649,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>520</v>
       </c>
@@ -11683,7 +11682,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>529</v>
       </c>
@@ -11716,7 +11715,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -11770,7 +11769,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -11911,7 +11910,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -12073,7 +12072,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -12126,7 +12125,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>521</v>
       </c>
@@ -12159,7 +12158,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>522</v>
       </c>
@@ -12192,7 +12191,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -12246,7 +12245,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -12300,7 +12299,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -12354,7 +12353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -12408,7 +12407,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -12516,7 +12515,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -12570,7 +12569,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -12624,7 +12623,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>526</v>
       </c>
@@ -12711,7 +12710,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -12981,7 +12980,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -13035,7 +13034,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -13089,7 +13088,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -13143,7 +13142,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -13197,7 +13196,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>528</v>
       </c>
@@ -13338,7 +13337,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -13392,7 +13391,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -13554,7 +13553,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -13695,7 +13694,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>524</v>
       </c>
@@ -13728,7 +13727,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -13782,7 +13781,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -13890,7 +13889,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -13944,7 +13943,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -14052,7 +14051,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -14106,7 +14105,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -14160,7 +14159,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -14214,7 +14213,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -14268,7 +14267,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -14376,7 +14375,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -14484,7 +14483,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -14538,7 +14537,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -14592,7 +14591,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -14700,7 +14699,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -14754,7 +14753,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -14949,7 +14948,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -15111,7 +15110,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -15165,7 +15164,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -15273,7 +15272,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -15381,7 +15380,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
         <v>498</v>
       </c>
@@ -15414,7 +15413,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -15468,7 +15467,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -15522,7 +15521,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -15630,7 +15629,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -15684,7 +15683,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -15738,7 +15737,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -15792,7 +15791,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -15846,7 +15845,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -15900,7 +15899,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -16008,7 +16007,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -16278,7 +16277,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -16332,7 +16331,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -16386,7 +16385,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -16494,7 +16493,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -16904,7 +16903,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -16958,7 +16957,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -17120,7 +17119,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>11</v>
       </c>
@@ -17224,7 +17223,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -17278,7 +17277,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -17332,7 +17331,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>11</v>
       </c>
@@ -17386,7 +17385,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -17440,7 +17439,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>11</v>
       </c>
@@ -17494,7 +17493,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="208" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -17656,7 +17655,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -17764,7 +17763,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>11</v>
       </c>
@@ -17818,7 +17817,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>11</v>
       </c>
@@ -17980,7 +17979,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>11</v>
       </c>
@@ -18034,7 +18033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -18088,7 +18087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>11</v>
       </c>
@@ -18142,7 +18141,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -18358,7 +18357,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>11</v>
       </c>
@@ -18412,7 +18411,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>11</v>
       </c>
@@ -18661,7 +18660,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="230" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>11</v>
       </c>
@@ -19147,7 +19146,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>11</v>
       </c>
@@ -19255,7 +19254,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="241" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>11</v>
       </c>
@@ -19309,7 +19308,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="242" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -19687,7 +19686,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="249" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>11</v>
       </c>
@@ -19741,7 +19740,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="250" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>11</v>
       </c>
@@ -19849,7 +19848,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="252" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B252" t="s">
         <v>536</v>
       </c>
@@ -19882,7 +19881,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="253" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>11</v>
       </c>
@@ -19936,7 +19935,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="254" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>11</v>
       </c>
@@ -19990,7 +19989,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="255" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>11</v>
       </c>
@@ -20044,7 +20043,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="256" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>11</v>
       </c>
@@ -20098,7 +20097,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="257" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>11</v>
       </c>
@@ -20152,7 +20151,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="258" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>11</v>
       </c>
@@ -20260,7 +20259,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="260" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>11</v>
       </c>
@@ -20422,7 +20421,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="263" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>11</v>
       </c>
@@ -20476,7 +20475,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="264" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B264" t="s">
         <v>530</v>
       </c>
@@ -20509,7 +20508,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="265" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>11</v>
       </c>
@@ -20670,7 +20669,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="268" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>11</v>
       </c>
@@ -20724,7 +20723,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="269" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>11</v>
       </c>
@@ -20886,7 +20885,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="272" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>11</v>
       </c>
@@ -20940,7 +20939,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="273" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>11</v>
       </c>
@@ -20994,7 +20993,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="274" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>11</v>
       </c>
@@ -21102,7 +21101,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="276" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>11</v>
       </c>
@@ -21156,7 +21155,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="277" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>11</v>
       </c>
@@ -21210,7 +21209,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="278" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>11</v>
       </c>
@@ -21264,7 +21263,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="279" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>11</v>
       </c>
@@ -21534,7 +21533,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="284" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>11</v>
       </c>
@@ -21588,7 +21587,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="285" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>11</v>
       </c>
@@ -21642,7 +21641,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="286" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>11</v>
       </c>
@@ -21696,7 +21695,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="287" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>11</v>
       </c>
@@ -21750,7 +21749,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="288" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>11</v>
       </c>
@@ -21964,7 +21963,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="292" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>11</v>
       </c>
@@ -22287,7 +22286,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="298" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>11</v>
       </c>
@@ -22501,7 +22500,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="302" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>11</v>
       </c>
@@ -22663,7 +22662,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="305" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B305" t="s">
         <v>532</v>
       </c>
@@ -22696,7 +22695,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="306" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B306" t="s">
         <v>533</v>
       </c>
@@ -22729,7 +22728,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="307" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B307" t="s">
         <v>534</v>
       </c>
@@ -22762,7 +22761,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="308" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B308" t="s">
         <v>535</v>
       </c>
@@ -22848,7 +22847,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="310" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>11</v>
       </c>
@@ -22902,7 +22901,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="311" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>11</v>
       </c>
@@ -22956,7 +22955,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="312" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>11</v>
       </c>
@@ -23010,7 +23009,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="313" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>11</v>
       </c>
@@ -23118,7 +23117,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="315" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>11</v>
       </c>
@@ -23762,7 +23761,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="327" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>11</v>
       </c>
@@ -23815,7 +23814,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="328" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>11</v>
       </c>
@@ -23922,7 +23921,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="330" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>11</v>
       </c>
@@ -23976,7 +23975,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="331" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>11</v>
       </c>
@@ -24030,7 +24029,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="332" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>11</v>
       </c>
@@ -24084,7 +24083,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="333" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>11</v>
       </c>
@@ -24138,7 +24137,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="334" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>11</v>
       </c>
@@ -24406,7 +24405,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="339" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>11</v>
       </c>
@@ -24460,7 +24459,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="340" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B340" t="s">
         <v>531</v>
       </c>
@@ -24493,7 +24492,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="341" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>11</v>
       </c>
@@ -24547,7 +24546,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="342" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>11</v>
       </c>
@@ -24601,7 +24600,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="343" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>11</v>
       </c>
@@ -24655,7 +24654,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="344" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>11</v>
       </c>
@@ -24709,7 +24708,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="345" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>11</v>
       </c>
@@ -24763,7 +24762,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="346" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>11</v>
       </c>
@@ -24817,7 +24816,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="347" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>11</v>
       </c>
@@ -25032,7 +25031,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="351" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>11</v>
       </c>
@@ -25192,7 +25191,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="354" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>11</v>
       </c>
@@ -25246,7 +25245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>11</v>
       </c>
@@ -25300,7 +25299,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="356" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>11</v>
       </c>
@@ -25354,7 +25353,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="357" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>11</v>
       </c>
@@ -25462,7 +25461,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="359" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>11</v>
       </c>
@@ -25516,7 +25515,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="360" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>11</v>
       </c>
@@ -25570,7 +25569,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="361" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>11</v>
       </c>
@@ -25624,7 +25623,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="362" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>11</v>
       </c>
@@ -25678,7 +25677,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="363" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>11</v>
       </c>
@@ -25731,7 +25730,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="364" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>11</v>
       </c>
@@ -25785,7 +25784,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="365" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>11</v>
       </c>
@@ -26001,7 +26000,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="369" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>11</v>
       </c>
@@ -26055,7 +26054,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="370" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>11</v>
       </c>
@@ -26109,7 +26108,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="371" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>11</v>
       </c>
@@ -26163,7 +26162,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="372" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>11</v>
       </c>
@@ -26217,7 +26216,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="373" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>11</v>
       </c>
@@ -26271,7 +26270,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="374" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>11</v>
       </c>
@@ -26325,7 +26324,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="375" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>11</v>
       </c>
@@ -26379,7 +26378,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="376" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>11</v>
       </c>
@@ -26433,7 +26432,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="377" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>11</v>
       </c>
@@ -26540,7 +26539,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="379" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>11</v>
       </c>
@@ -26594,7 +26593,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="380" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>11</v>
       </c>
@@ -26754,7 +26753,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="383" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B383" t="s">
         <v>504</v>
       </c>
@@ -26820,7 +26819,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="385" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>11</v>
       </c>
@@ -26873,7 +26872,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="386" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>11</v>
       </c>
@@ -26926,7 +26925,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="387" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>11</v>
       </c>
@@ -26979,7 +26978,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="388" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>11</v>
       </c>
@@ -27033,7 +27032,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="389" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>11</v>
       </c>
@@ -27087,7 +27086,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="390" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>11</v>
       </c>
@@ -27194,7 +27193,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="392" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>11</v>
       </c>
@@ -27247,7 +27246,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="393" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>11</v>
       </c>
@@ -27301,7 +27300,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="394" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>11</v>
       </c>
@@ -27355,7 +27354,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="395" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>11</v>
       </c>
@@ -27409,7 +27408,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="396" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>11</v>
       </c>
@@ -27463,7 +27462,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="397" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>11</v>
       </c>
@@ -27679,7 +27678,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="401" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>11</v>
       </c>
@@ -27733,7 +27732,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="402" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>11</v>
       </c>
@@ -27787,7 +27786,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="403" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>11</v>
       </c>
@@ -27841,7 +27840,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="404" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>11</v>
       </c>
@@ -27895,7 +27894,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="405" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>11</v>
       </c>
@@ -27949,7 +27948,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="406" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>11</v>
       </c>
@@ -28003,7 +28002,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="407" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>11</v>
       </c>
@@ -28057,7 +28056,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="408" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>11</v>
       </c>
@@ -28111,7 +28110,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="409" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>11</v>
       </c>
@@ -28219,7 +28218,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="411" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>11</v>
       </c>
@@ -28273,7 +28272,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="412" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>11</v>
       </c>
@@ -28327,7 +28326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>11</v>
       </c>
@@ -28489,7 +28488,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="416" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>11</v>
       </c>
@@ -28543,7 +28542,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="417" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>11</v>
       </c>
@@ -28705,7 +28704,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="420" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>11</v>
       </c>
@@ -28759,7 +28758,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="421" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>11</v>
       </c>
@@ -28813,7 +28812,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="422" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>11</v>
       </c>
@@ -28921,7 +28920,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="424" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>11</v>
       </c>
@@ -28975,7 +28974,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="425" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>11</v>
       </c>
@@ -29029,7 +29028,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="426" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>11</v>
       </c>
@@ -29083,7 +29082,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="427" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>11</v>
       </c>
@@ -29299,7 +29298,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="431" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>11</v>
       </c>
@@ -29353,7 +29352,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="432" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>11</v>
       </c>
@@ -29407,7 +29406,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="433" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>11</v>
       </c>
@@ -29461,7 +29460,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="434" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>11</v>
       </c>
@@ -29569,7 +29568,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="436" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>11</v>
       </c>
@@ -29623,7 +29622,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="437" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>11</v>
       </c>
@@ -29677,7 +29676,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="438" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>11</v>
       </c>
@@ -29731,7 +29730,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="439" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B439" t="s">
         <v>540</v>
       </c>
@@ -29764,7 +29763,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="440" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>11</v>
       </c>
@@ -29818,7 +29817,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="441" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>11</v>
       </c>
@@ -29872,7 +29871,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="442" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>11</v>
       </c>
@@ -29926,7 +29925,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="443" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>11</v>
       </c>
@@ -29980,7 +29979,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="444" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>11</v>
       </c>
@@ -30034,7 +30033,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="445" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>11</v>
       </c>
@@ -30088,7 +30087,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="446" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>11</v>
       </c>
@@ -30142,7 +30141,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="447" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>11</v>
       </c>
@@ -30196,7 +30195,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="448" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>11</v>
       </c>
@@ -30250,7 +30249,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="449" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B449" t="s">
         <v>542</v>
       </c>
@@ -30283,7 +30282,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="450" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B450" t="s">
         <v>543</v>
       </c>
@@ -30316,7 +30315,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="451" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>11</v>
       </c>
@@ -30478,7 +30477,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="454" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B454" t="s">
         <v>541</v>
       </c>
@@ -30511,7 +30510,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="455" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B455" t="s">
         <v>544</v>
       </c>
@@ -30544,7 +30543,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="456" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B456" t="s">
         <v>545</v>
       </c>
@@ -30577,7 +30576,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="457" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B457" t="s">
         <v>546</v>
       </c>
@@ -30610,7 +30609,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="458" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B458" t="s">
         <v>547</v>
       </c>
@@ -30643,7 +30642,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="459" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B459" t="s">
         <v>548</v>
       </c>
@@ -30676,7 +30675,7 @@
         <v>KEEP</v>
       </c>
     </row>
-    <row r="460" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>11</v>
       </c>
@@ -30784,7 +30783,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="462" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B462" t="s">
         <v>539</v>
       </c>
@@ -30871,7 +30870,7 @@
         <v>PHASE OUT</v>
       </c>
     </row>
-    <row r="464" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>11</v>
       </c>
@@ -30932,18 +30931,7 @@
       <c r="H468" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R464" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Oil"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="17">
-      <filters>
-        <filter val="PHASE OUT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R464" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A290:O409">
     <sortCondition ref="N290:N464"/>
   </sortState>

</xml_diff>